<commit_message>
Updated Simulated Annealing (Had an issue where it wasnt' accepting worse moves) as well as adding plotting
</commit_message>
<xml_diff>
--- a/optimized_routes.xlsx
+++ b/optimized_routes.xlsx
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>43</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>35</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>29</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>46</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8">
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>82</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>89</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10">
@@ -546,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
@@ -557,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12">
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13">
@@ -579,7 +579,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15">
@@ -601,7 +601,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>102</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -612,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17">
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>94</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>97</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19">
@@ -645,7 +645,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20">
@@ -656,7 +656,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21">
@@ -667,7 +667,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -678,7 +678,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -700,7 +700,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25">
@@ -711,7 +711,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26">
@@ -722,7 +722,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
@@ -733,7 +733,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28">
@@ -744,7 +744,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
@@ -755,7 +755,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
@@ -766,7 +766,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -777,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>44</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
@@ -788,7 +788,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33">
@@ -810,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="n">
-        <v>85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
@@ -821,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="n">
-        <v>81</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36">
@@ -832,7 +832,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>95</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37">
@@ -843,7 +843,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="n">
-        <v>88</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38">
@@ -854,7 +854,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="n">
-        <v>87</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39">
@@ -865,7 +865,7 @@
         <v>7</v>
       </c>
       <c r="C39" t="n">
-        <v>112</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40">
@@ -876,7 +876,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41">
@@ -887,7 +887,7 @@
         <v>9</v>
       </c>
       <c r="C41" t="n">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42">
@@ -898,7 +898,7 @@
         <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43">
@@ -909,7 +909,7 @@
         <v>11</v>
       </c>
       <c r="C43" t="n">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44">
@@ -920,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="C44" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45">
@@ -931,7 +931,7 @@
         <v>13</v>
       </c>
       <c r="C45" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
@@ -942,7 +942,7 @@
         <v>14</v>
       </c>
       <c r="C46" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
@@ -953,7 +953,7 @@
         <v>15</v>
       </c>
       <c r="C47" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48">
@@ -964,7 +964,7 @@
         <v>16</v>
       </c>
       <c r="C48" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49">
@@ -975,7 +975,7 @@
         <v>17</v>
       </c>
       <c r="C49" t="n">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50">
@@ -986,7 +986,7 @@
         <v>18</v>
       </c>
       <c r="C50" t="n">
-        <v>15</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51">
@@ -997,7 +997,7 @@
         <v>19</v>
       </c>
       <c r="C51" t="n">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52">
@@ -1008,7 +1008,7 @@
         <v>20</v>
       </c>
       <c r="C52" t="n">
-        <v>4</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53">
@@ -1019,7 +1019,7 @@
         <v>21</v>
       </c>
       <c r="C53" t="n">
-        <v>23</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54">
@@ -1030,7 +1030,7 @@
         <v>22</v>
       </c>
       <c r="C54" t="n">
-        <v>27</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55">
@@ -1041,7 +1041,7 @@
         <v>23</v>
       </c>
       <c r="C55" t="n">
-        <v>31</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56">
@@ -1052,7 +1052,7 @@
         <v>24</v>
       </c>
       <c r="C56" t="n">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57">
@@ -1063,7 +1063,7 @@
         <v>25</v>
       </c>
       <c r="C57" t="n">
-        <v>61</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58">
@@ -1074,7 +1074,7 @@
         <v>26</v>
       </c>
       <c r="C58" t="n">
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59">
@@ -1085,7 +1085,7 @@
         <v>27</v>
       </c>
       <c r="C59" t="n">
-        <v>74</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60">
@@ -1096,7 +1096,7 @@
         <v>28</v>
       </c>
       <c r="C60" t="n">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61">
@@ -1107,7 +1107,7 @@
         <v>29</v>
       </c>
       <c r="C61" t="n">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62">
@@ -1118,7 +1118,7 @@
         <v>30</v>
       </c>
       <c r="C62" t="n">
-        <v>110</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63">
@@ -1129,7 +1129,7 @@
         <v>31</v>
       </c>
       <c r="C63" t="n">
-        <v>111</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64">
@@ -1151,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="C65" t="n">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66">
@@ -1162,7 +1162,7 @@
         <v>3</v>
       </c>
       <c r="C66" t="n">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67">
@@ -1173,7 +1173,7 @@
         <v>4</v>
       </c>
       <c r="C67" t="n">
-        <v>96</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68">
@@ -1184,7 +1184,7 @@
         <v>5</v>
       </c>
       <c r="C68" t="n">
-        <v>104</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69">
@@ -1195,7 +1195,7 @@
         <v>6</v>
       </c>
       <c r="C69" t="n">
-        <v>108</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70">
@@ -1206,7 +1206,7 @@
         <v>7</v>
       </c>
       <c r="C70" t="n">
-        <v>116</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71">
@@ -1217,7 +1217,7 @@
         <v>8</v>
       </c>
       <c r="C71" t="n">
-        <v>115</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72">
@@ -1228,7 +1228,7 @@
         <v>9</v>
       </c>
       <c r="C72" t="n">
-        <v>113</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73">
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="C73" t="n">
-        <v>105</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74">
@@ -1250,7 +1250,7 @@
         <v>11</v>
       </c>
       <c r="C74" t="n">
-        <v>98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -1261,7 +1261,7 @@
         <v>12</v>
       </c>
       <c r="C75" t="n">
-        <v>92</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
@@ -1272,7 +1272,7 @@
         <v>13</v>
       </c>
       <c r="C76" t="n">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77">
@@ -1283,7 +1283,7 @@
         <v>14</v>
       </c>
       <c r="C77" t="n">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78">
@@ -1294,7 +1294,7 @@
         <v>15</v>
       </c>
       <c r="C78" t="n">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="79">
@@ -1305,7 +1305,7 @@
         <v>16</v>
       </c>
       <c r="C79" t="n">
-        <v>56</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80">
@@ -1316,7 +1316,7 @@
         <v>17</v>
       </c>
       <c r="C80" t="n">
-        <v>49</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81">
@@ -1327,7 +1327,7 @@
         <v>18</v>
       </c>
       <c r="C81" t="n">
-        <v>51</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82">
@@ -1338,7 +1338,7 @@
         <v>19</v>
       </c>
       <c r="C82" t="n">
-        <v>59</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83">
@@ -1349,7 +1349,7 @@
         <v>20</v>
       </c>
       <c r="C83" t="n">
-        <v>68</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84">
@@ -1360,7 +1360,7 @@
         <v>21</v>
       </c>
       <c r="C84" t="n">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85">
@@ -1382,7 +1382,7 @@
         <v>23</v>
       </c>
       <c r="C86" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87">
@@ -1393,7 +1393,7 @@
         <v>24</v>
       </c>
       <c r="C87" t="n">
-        <v>25</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88">
@@ -1404,7 +1404,7 @@
         <v>25</v>
       </c>
       <c r="C88" t="n">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="89">
@@ -1415,7 +1415,7 @@
         <v>26</v>
       </c>
       <c r="C89" t="n">
-        <v>9</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90">
@@ -1426,7 +1426,7 @@
         <v>27</v>
       </c>
       <c r="C90" t="n">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91">
@@ -1437,7 +1437,7 @@
         <v>28</v>
       </c>
       <c r="C91" t="n">
-        <v>32</v>
+        <v>78</v>
       </c>
     </row>
     <row r="92">
@@ -1448,7 +1448,7 @@
         <v>29</v>
       </c>
       <c r="C92" t="n">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93">
@@ -1459,7 +1459,7 @@
         <v>30</v>
       </c>
       <c r="C93" t="n">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="94">
@@ -1470,7 +1470,7 @@
         <v>31</v>
       </c>
       <c r="C94" t="n">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="95">
@@ -1492,7 +1492,7 @@
         <v>2</v>
       </c>
       <c r="C96" t="n">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97">
@@ -1503,7 +1503,7 @@
         <v>3</v>
       </c>
       <c r="C97" t="n">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98">
@@ -1514,7 +1514,7 @@
         <v>4</v>
       </c>
       <c r="C98" t="n">
-        <v>77</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99">
@@ -1525,7 +1525,7 @@
         <v>5</v>
       </c>
       <c r="C99" t="n">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100">
@@ -1536,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="C100" t="n">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101">
@@ -1547,7 +1547,7 @@
         <v>7</v>
       </c>
       <c r="C101" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102">
@@ -1558,7 +1558,7 @@
         <v>8</v>
       </c>
       <c r="C102" t="n">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="103">
@@ -1569,7 +1569,7 @@
         <v>9</v>
       </c>
       <c r="C103" t="n">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104">
@@ -1580,7 +1580,7 @@
         <v>10</v>
       </c>
       <c r="C104" t="n">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="105">
@@ -1591,7 +1591,7 @@
         <v>11</v>
       </c>
       <c r="C105" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="106">
@@ -1602,7 +1602,7 @@
         <v>12</v>
       </c>
       <c r="C106" t="n">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="107">
@@ -1613,7 +1613,7 @@
         <v>13</v>
       </c>
       <c r="C107" t="n">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="108">
@@ -1624,7 +1624,7 @@
         <v>14</v>
       </c>
       <c r="C108" t="n">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="109">
@@ -1635,7 +1635,7 @@
         <v>15</v>
       </c>
       <c r="C109" t="n">
-        <v>64</v>
+        <v>92</v>
       </c>
     </row>
     <row r="110">
@@ -1646,7 +1646,7 @@
         <v>16</v>
       </c>
       <c r="C110" t="n">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111">
@@ -1657,7 +1657,7 @@
         <v>17</v>
       </c>
       <c r="C111" t="n">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="112">
@@ -1668,7 +1668,7 @@
         <v>18</v>
       </c>
       <c r="C112" t="n">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
     <row r="113">
@@ -1679,7 +1679,7 @@
         <v>19</v>
       </c>
       <c r="C113" t="n">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="114">
@@ -1690,7 +1690,7 @@
         <v>20</v>
       </c>
       <c r="C114" t="n">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="115">
@@ -1701,7 +1701,7 @@
         <v>21</v>
       </c>
       <c r="C115" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="116">
@@ -1712,7 +1712,7 @@
         <v>22</v>
       </c>
       <c r="C116" t="n">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="117">
@@ -1723,7 +1723,7 @@
         <v>23</v>
       </c>
       <c r="C117" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="118">
@@ -1734,7 +1734,7 @@
         <v>24</v>
       </c>
       <c r="C118" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="119">
@@ -1745,7 +1745,7 @@
         <v>25</v>
       </c>
       <c r="C119" t="n">
-        <v>24</v>
+        <v>75</v>
       </c>
     </row>
     <row r="120">
@@ -1756,7 +1756,7 @@
         <v>26</v>
       </c>
       <c r="C120" t="n">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="121">
@@ -1767,7 +1767,7 @@
         <v>27</v>
       </c>
       <c r="C121" t="n">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122">
@@ -1778,7 +1778,7 @@
         <v>28</v>
       </c>
       <c r="C122" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="123">
@@ -1789,7 +1789,7 @@
         <v>29</v>
       </c>
       <c r="C123" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124">
@@ -1800,7 +1800,7 @@
         <v>30</v>
       </c>
       <c r="C124" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
@@ -1811,7 +1811,7 @@
         <v>31</v>
       </c>
       <c r="C125" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added intra route which fixed the largest issue in previous code
</commit_message>
<xml_diff>
--- a/optimized_routes.xlsx
+++ b/optimized_routes.xlsx
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8">
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>82</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
@@ -546,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11">
@@ -557,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13">
@@ -579,7 +579,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14">
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15">
@@ -601,7 +601,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16">
@@ -612,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17">
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -645,7 +645,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
@@ -656,7 +656,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21">
@@ -667,7 +667,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
@@ -678,7 +678,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -689,7 +689,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24">
@@ -700,7 +700,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>113</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25">
@@ -711,7 +711,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>109</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
@@ -722,7 +722,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27">
@@ -733,7 +733,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>96</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28">
@@ -755,18 +755,18 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>112</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31">
@@ -774,10 +774,10 @@
         <v>2</v>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -785,10 +785,10 @@
         <v>2</v>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="n">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33">
@@ -796,10 +796,10 @@
         <v>2</v>
       </c>
       <c r="B33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" t="n">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34">
@@ -807,10 +807,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35">
@@ -818,10 +818,10 @@
         <v>2</v>
       </c>
       <c r="B35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36">
@@ -829,10 +829,10 @@
         <v>2</v>
       </c>
       <c r="B36" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" t="n">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37">
@@ -840,10 +840,10 @@
         <v>2</v>
       </c>
       <c r="B37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38">
@@ -851,10 +851,10 @@
         <v>2</v>
       </c>
       <c r="B38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" t="n">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39">
@@ -862,10 +862,10 @@
         <v>2</v>
       </c>
       <c r="B39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" t="n">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40">
@@ -873,10 +873,10 @@
         <v>2</v>
       </c>
       <c r="B40" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C40" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41">
@@ -884,10 +884,10 @@
         <v>2</v>
       </c>
       <c r="B41" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C41" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42">
@@ -895,10 +895,10 @@
         <v>2</v>
       </c>
       <c r="B42" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C42" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43">
@@ -906,10 +906,10 @@
         <v>2</v>
       </c>
       <c r="B43" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C43" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44">
@@ -917,10 +917,10 @@
         <v>2</v>
       </c>
       <c r="B44" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44" t="n">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45">
@@ -928,10 +928,10 @@
         <v>2</v>
       </c>
       <c r="B45" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C45" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46">
@@ -939,10 +939,10 @@
         <v>2</v>
       </c>
       <c r="B46" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C46" t="n">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47">
@@ -950,10 +950,10 @@
         <v>2</v>
       </c>
       <c r="B47" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" t="n">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48">
@@ -961,10 +961,10 @@
         <v>2</v>
       </c>
       <c r="B48" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C48" t="n">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49">
@@ -972,10 +972,10 @@
         <v>2</v>
       </c>
       <c r="B49" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C49" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50">
@@ -983,10 +983,10 @@
         <v>2</v>
       </c>
       <c r="B50" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C50" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51">
@@ -994,10 +994,10 @@
         <v>2</v>
       </c>
       <c r="B51" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C51" t="n">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52">
@@ -1005,10 +1005,10 @@
         <v>2</v>
       </c>
       <c r="B52" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C52" t="n">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53">
@@ -1016,10 +1016,10 @@
         <v>2</v>
       </c>
       <c r="B53" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C53" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54">
@@ -1027,10 +1027,10 @@
         <v>2</v>
       </c>
       <c r="B54" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C54" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55">
@@ -1038,10 +1038,10 @@
         <v>2</v>
       </c>
       <c r="B55" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C55" t="n">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56">
@@ -1049,10 +1049,10 @@
         <v>2</v>
       </c>
       <c r="B56" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C56" t="n">
-        <v>56</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57">
@@ -1060,10 +1060,10 @@
         <v>2</v>
       </c>
       <c r="B57" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C57" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58">
@@ -1071,10 +1071,10 @@
         <v>2</v>
       </c>
       <c r="B58" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C58" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59">
@@ -1082,10 +1082,10 @@
         <v>2</v>
       </c>
       <c r="B59" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C59" t="n">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60">
@@ -1093,10 +1093,10 @@
         <v>2</v>
       </c>
       <c r="B60" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C60" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61">
@@ -1104,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="B61" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C61" t="n">
         <v>39</v>
@@ -1115,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C62" t="n">
         <v>47</v>
@@ -1126,7 +1126,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C63" t="n">
         <v>48</v>
@@ -1137,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="B64" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C64" t="n">
         <v>40</v>
@@ -1148,7 +1148,7 @@
         <v>2</v>
       </c>
       <c r="B65" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C65" t="n">
         <v>38</v>
@@ -1159,10 +1159,10 @@
         <v>2</v>
       </c>
       <c r="B66" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C66" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67">
@@ -1170,10 +1170,10 @@
         <v>2</v>
       </c>
       <c r="B67" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C67" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68">
@@ -1181,10 +1181,10 @@
         <v>2</v>
       </c>
       <c r="B68" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C68" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
@@ -1192,10 +1192,10 @@
         <v>2</v>
       </c>
       <c r="B69" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -1203,10 +1203,10 @@
         <v>2</v>
       </c>
       <c r="B70" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C70" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -1214,10 +1214,10 @@
         <v>2</v>
       </c>
       <c r="B71" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C71" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72">
@@ -1225,21 +1225,21 @@
         <v>2</v>
       </c>
       <c r="B72" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C72" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B73" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="C73" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1247,10 +1247,10 @@
         <v>3</v>
       </c>
       <c r="B74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75">
@@ -1258,10 +1258,10 @@
         <v>3</v>
       </c>
       <c r="B75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75" t="n">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76">
@@ -1269,10 +1269,10 @@
         <v>3</v>
       </c>
       <c r="B76" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C76" t="n">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77">
@@ -1280,10 +1280,10 @@
         <v>3</v>
       </c>
       <c r="B77" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C77" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78">
@@ -1291,10 +1291,10 @@
         <v>3</v>
       </c>
       <c r="B78" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C78" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="79">
@@ -1302,10 +1302,10 @@
         <v>3</v>
       </c>
       <c r="B79" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C79" t="n">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80">
@@ -1313,10 +1313,10 @@
         <v>3</v>
       </c>
       <c r="B80" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C80" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="81">
@@ -1324,10 +1324,10 @@
         <v>3</v>
       </c>
       <c r="B81" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C81" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82">
@@ -1335,10 +1335,10 @@
         <v>3</v>
       </c>
       <c r="B82" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C82" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83">
@@ -1346,10 +1346,10 @@
         <v>3</v>
       </c>
       <c r="B83" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C83" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84">
@@ -1357,10 +1357,10 @@
         <v>3</v>
       </c>
       <c r="B84" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C84" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85">
@@ -1368,10 +1368,10 @@
         <v>3</v>
       </c>
       <c r="B85" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C85" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86">
@@ -1379,10 +1379,10 @@
         <v>3</v>
       </c>
       <c r="B86" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C86" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87">
@@ -1390,10 +1390,10 @@
         <v>3</v>
       </c>
       <c r="B87" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C87" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88">
@@ -1401,10 +1401,10 @@
         <v>3</v>
       </c>
       <c r="B88" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C88" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89">
@@ -1412,10 +1412,10 @@
         <v>3</v>
       </c>
       <c r="B89" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C89" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90">
@@ -1423,10 +1423,10 @@
         <v>3</v>
       </c>
       <c r="B90" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C90" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91">
@@ -1434,10 +1434,10 @@
         <v>3</v>
       </c>
       <c r="B91" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C91" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92">
@@ -1445,10 +1445,10 @@
         <v>3</v>
       </c>
       <c r="B92" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C92" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93">
@@ -1456,10 +1456,10 @@
         <v>3</v>
       </c>
       <c r="B93" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C93" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94">
@@ -1467,10 +1467,10 @@
         <v>3</v>
       </c>
       <c r="B94" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C94" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95">
@@ -1478,10 +1478,10 @@
         <v>3</v>
       </c>
       <c r="B95" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C95" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96">
@@ -1489,10 +1489,10 @@
         <v>3</v>
       </c>
       <c r="B96" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C96" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97">
@@ -1500,10 +1500,10 @@
         <v>3</v>
       </c>
       <c r="B97" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C97" t="n">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="98">
@@ -1511,10 +1511,10 @@
         <v>3</v>
       </c>
       <c r="B98" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C98" t="n">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99">
@@ -1522,10 +1522,10 @@
         <v>3</v>
       </c>
       <c r="B99" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C99" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="100">
@@ -1533,10 +1533,10 @@
         <v>3</v>
       </c>
       <c r="B100" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C100" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="101">
@@ -1544,10 +1544,10 @@
         <v>3</v>
       </c>
       <c r="B101" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C101" t="n">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102">
@@ -1555,10 +1555,10 @@
         <v>3</v>
       </c>
       <c r="B102" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C102" t="n">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="103">
@@ -1566,10 +1566,10 @@
         <v>3</v>
       </c>
       <c r="B103" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C103" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104">
@@ -1577,10 +1577,10 @@
         <v>3</v>
       </c>
       <c r="B104" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C104" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105">
@@ -1588,10 +1588,10 @@
         <v>3</v>
       </c>
       <c r="B105" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C105" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="106">
@@ -1599,10 +1599,10 @@
         <v>3</v>
       </c>
       <c r="B106" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C106" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107">
@@ -1610,10 +1610,10 @@
         <v>3</v>
       </c>
       <c r="B107" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C107" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108">
@@ -1621,10 +1621,10 @@
         <v>3</v>
       </c>
       <c r="B108" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C108" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109">
@@ -1632,32 +1632,32 @@
         <v>3</v>
       </c>
       <c r="B109" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C109" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B110" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C110" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B111" t="n">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="C111" t="n">
-        <v>1</v>
+        <v>81</v>
       </c>
     </row>
     <row r="112">
@@ -1665,10 +1665,10 @@
         <v>4</v>
       </c>
       <c r="B112" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C112" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="113">
@@ -1676,10 +1676,10 @@
         <v>4</v>
       </c>
       <c r="B113" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C113" t="n">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="114">
@@ -1687,10 +1687,10 @@
         <v>4</v>
       </c>
       <c r="B114" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C114" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="115">
@@ -1698,10 +1698,10 @@
         <v>4</v>
       </c>
       <c r="B115" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C115" t="n">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="116">
@@ -1709,10 +1709,10 @@
         <v>4</v>
       </c>
       <c r="B116" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C116" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117">
@@ -1720,10 +1720,10 @@
         <v>4</v>
       </c>
       <c r="B117" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C117" t="n">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="118">
@@ -1731,10 +1731,10 @@
         <v>4</v>
       </c>
       <c r="B118" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C118" t="n">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="119">
@@ -1742,7 +1742,7 @@
         <v>4</v>
       </c>
       <c r="B119" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C119" t="n">
         <v>57</v>
@@ -1753,10 +1753,10 @@
         <v>4</v>
       </c>
       <c r="B120" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C120" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121">
@@ -1764,10 +1764,10 @@
         <v>4</v>
       </c>
       <c r="B121" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C121" t="n">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="122">
@@ -1775,10 +1775,10 @@
         <v>4</v>
       </c>
       <c r="B122" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C122" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="123">
@@ -1786,10 +1786,10 @@
         <v>4</v>
       </c>
       <c r="B123" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C123" t="n">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="124">
@@ -1797,10 +1797,10 @@
         <v>4</v>
       </c>
       <c r="B124" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C124" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="125">
@@ -1808,7 +1808,7 @@
         <v>4</v>
       </c>
       <c r="B125" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C125" t="n">
         <v>46</v>

</xml_diff>